<commit_message>
Update README and support dynamic designator and collection_url
</commit_message>
<xml_diff>
--- a/templates/sample.xlsx
+++ b/templates/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelbaylis/Dropbox/BiblicalStory/Development/testfolder2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelbaylis/Dropbox/BiblicalStory/Development/synapseconvert/synapseconvert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3527E3-1584-194A-B1FE-E1C070AA8757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002E0CDF-DE3A-4F4E-AA8E-82FBF4A87B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37500" yWindow="-3720" windowWidth="34560" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>collection</t>
   </si>
@@ -50,6 +50,54 @@
   </si>
   <si>
     <t>ris</t>
+  </si>
+  <si>
+    <t>designator</t>
+  </si>
+  <si>
+    <t>collection_url</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>thiscollection.org</t>
+  </si>
+  <si>
+    <t>firstcategory</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>categorical article</t>
+  </si>
+  <si>
+    <t>categoricalarticle.com</t>
+  </si>
+  <si>
+    <t>Tom Cat</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>2/52/2222</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>accompanyingsong.mp3</t>
+  </si>
+  <si>
+    <t>this collection</t>
+  </si>
+  <si>
+    <t>["cats", "categories", "Tom Cat"]</t>
+  </si>
+  <si>
+    <t>catfile.ris</t>
   </si>
 </sst>
 </file>
@@ -413,44 +461,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>